<commit_message>
update protocol for image
</commit_message>
<xml_diff>
--- a/任务表（持续更新）.xlsx
+++ b/任务表（持续更新）.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CSpractice\Wenochat\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B9E07F-A4E3-4D48-9146-0ABAFF8ADF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D72655F-6E8B-43F4-9E4E-E6C929D0E4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3497" yWindow="309" windowWidth="24686" windowHeight="16105" xr2:uid="{4D1AA702-3792-4D4F-A0C6-11D3DE3315D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4D1AA702-3792-4D4F-A0C6-11D3DE3315D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>1.初始版本</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -175,6 +175,42 @@
   </si>
   <si>
     <t>2.对话显示设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.好友列表（客户端）+消息记录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.封装对话框部分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zjk&amp;dzm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.头像系统-客户端zjk+服务端dzm+头像协议</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>传输方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>协议</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户端双socket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务端头像截取Qimage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.问题下拉框+找回密码部分能看美化+设计概要书</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -203,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +282,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -261,7 +303,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -287,6 +329,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -305,6 +362,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -624,20 +684,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB4FDA1C-7EC6-49CC-84CA-6DEC5E07B455}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E24"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="57" customWidth="1"/>
-    <col min="5" max="5" width="26.2109375" customWidth="1"/>
+    <col min="5" max="5" width="26.21875" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -654,11 +716,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="18">
         <v>8.18</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -667,48 +729,48 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="18">
         <v>8.19</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -717,95 +779,95 @@
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
-      <c r="B7" s="13"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
-      <c r="B8" s="13"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="1" t="s">
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="14"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="4" t="s">
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="5" t="s">
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="9" t="s">
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="4" t="s">
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15">
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="21">
         <v>8.1999999999999993</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -814,108 +876,157 @@
       <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="4" t="s">
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="15"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="18">
         <v>8.2100000000000009</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="10"/>
-      <c r="B21" s="2">
+      <c r="C20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10">
         <v>8.2200000000000006</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B25" s="2">
         <v>8.23</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="11"/>
-      <c r="B23" s="2">
+      <c r="C25" s="8"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="2">
         <v>8.24</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B27" s="2">
         <v>8.25</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="9"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="E2:E24"/>
+  <mergeCells count="11">
+    <mergeCell ref="E2:E27"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A26"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A6:A18"/>
@@ -923,6 +1034,7 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B20:B23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>